<commit_message>
Fixed a bug in the appendix (GJ vs. MJ).
</commit_message>
<xml_diff>
--- a/doc/appendix/Abschaetzung.xlsx
+++ b/doc/appendix/Abschaetzung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\FHNW\glaL4-SimTools-SwimmingPoolSimulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\SwimmingPoolSimulation\doc\appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FF877C-5758-4C56-97DB-3B673A0CBCB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F1614A-9690-4D20-A9A2-D14ED3340D63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>IST-Temperatur:</t>
   </si>
@@ -96,9 +96,6 @@
     <t>(s)</t>
   </si>
   <si>
-    <t>MJ</t>
-  </si>
-  <si>
     <t>Abschätzung</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Umwälzzeit:</t>
+  </si>
+  <si>
+    <t>GJ</t>
   </si>
 </sst>
 </file>
@@ -113,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -227,29 +227,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -278,8 +278,8 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="430439" cy="378180"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="Textfeld 3">
@@ -374,7 +374,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="Textfeld 3">
@@ -452,8 +452,8 @@
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739113" cy="187872"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="Textfeld 4">
@@ -548,7 +548,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="Textfeld 4">
@@ -633,8 +633,8 @@
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1291443" cy="187872"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="Textfeld 5">
@@ -782,7 +782,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="Textfeld 5">
@@ -848,8 +848,8 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="412612" cy="345672"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="Textfeld 7">
@@ -943,7 +943,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="Textfeld 7">
@@ -1008,8 +1008,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="294055" cy="349648"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="Textfeld 6">
@@ -1102,7 +1102,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="Textfeld 6">
@@ -1191,8 +1191,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="664028" cy="187872"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="Textfeld 6">
@@ -1280,7 +1280,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="Textfeld 6">
@@ -1358,8 +1358,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128881" cy="349519"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Textfeld 3">
@@ -1411,7 +1411,7 @@
                     <m:f>
                       <m:fPr>
                         <m:ctrlPr>
-                          <a:rPr lang="de-CH" sz="1200" b="1" i="0">
+                          <a:rPr lang="de-CH" sz="1200" b="1" i="1">
                             <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
@@ -1441,7 +1441,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="Textfeld 3">
@@ -1793,44 +1793,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="3">
         <v>4</v>
       </c>
@@ -1838,41 +1838,41 @@
         <v>9</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="14"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="3">
         <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="5">
         <f>E16/48</f>
         <v>1012.4999999999999</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1881,56 +1881,56 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="H11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="21">
+      <c r="H12" s="17">
         <f>E15*E7/3600*E5</f>
         <v>4706.9999999999991</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <f>IF(COUNT(E16,E15,E14,E13)=4,ROUND(E16*E15*(E14-E13),0),"")</f>
         <v>4066848000</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="21">
+      <c r="J12" s="21"/>
+      <c r="K12" s="17">
         <f>IF(COUNT(I12,H12)=2,ROUNDDOWN((I12/H12)/86400,0),"")</f>
         <v>10</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="17">
         <f>IF(COUNT(I12,H12)=2,IF(ROUND((I12/H12)-(K12*60),0)=60,1,0),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="3">
         <v>10</v>
       </c>
@@ -1938,11 +1938,11 @@
         <v>4</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="5">
         <f>IF(COUNT(L12=1),IF(L12=1,K12+1,K12),"")</f>
         <v>10</v>
@@ -1952,11 +1952,11 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="3">
         <v>30</v>
       </c>
@@ -1974,38 +1974,38 @@
       <c r="O14" s="12"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="3">
         <v>4184</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="19">
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="15">
         <f>I12/1000000000</f>
         <v>4.0668480000000002</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="3">
         <f>8.1*4*1.5*1000</f>
         <v>48599.999999999993</v>
@@ -2014,17 +2014,17 @@
         <v>3</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="19">
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="15">
         <f>H12/1000</f>
         <v>4.706999999999999</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -2038,7 +2038,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:K1"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B15:D15"/>
@@ -2053,11 +2052,12 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated documentation, added electrical heater.
</commit_message>
<xml_diff>
--- a/doc/appendix/Abschaetzung.xlsx
+++ b/doc/appendix/Abschaetzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\SwimmingPoolSimulation\doc\appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F1614A-9690-4D20-A9A2-D14ED3340D63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D66AEA6-859F-4B26-AAE8-1BB7D9B27262}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,20 +236,20 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1793,37 +1793,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
       <c r="L1" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
@@ -1832,7 +1832,7 @@
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -1888,37 +1888,37 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H12" s="17">
         <f>E15*E7/3600*E5</f>
-        <v>4706.9999999999991</v>
-      </c>
-      <c r="I12" s="21">
+        <v>3530.2499999999991</v>
+      </c>
+      <c r="I12" s="18">
         <f>IF(COUNT(E16,E15,E14,E13)=4,ROUND(E16*E15*(E14-E13),0),"")</f>
         <v>4066848000</v>
       </c>
-      <c r="J12" s="21"/>
+      <c r="J12" s="18"/>
       <c r="K12" s="17">
         <f>IF(COUNT(I12,H12)=2,ROUNDDOWN((I12/H12)/86400,0),"")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L12" s="17">
         <f>IF(COUNT(I12,H12)=2,IF(ROUND((I12/H12)-(K12*60),0)=60,1,0),"")</f>
@@ -1945,18 +1945,18 @@
       <c r="J13" s="19"/>
       <c r="K13" s="5">
         <f>IF(COUNT(L12=1),IF(L12=1,K12+1,K12),"")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="3">
         <v>30</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="G14" s="2"/>
       <c r="K14" s="5">
         <f>IF(COUNT(K13)=1,IF(ROUND(((I12/H12)-(K13*86400))/3600,0)=60,0,((I12/H12)-(K13*86400)))/3600,"")</f>
-        <v>3.2337589396370782E-14</v>
+        <v>8.0000000000000639</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>14</v>
@@ -2021,7 +2021,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="15">
         <f>H12/1000</f>
-        <v>4.706999999999999</v>
+        <v>3.5302499999999992</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>22</v>
@@ -2038,6 +2038,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B15:D15"/>
@@ -2052,12 +2058,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on the documentation.
</commit_message>
<xml_diff>
--- a/doc/appendix/Abschaetzung.xlsx
+++ b/doc/appendix/Abschaetzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\SwimmingPoolSimulation\doc\appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D66AEA6-859F-4B26-AAE8-1BB7D9B27262}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2EDA93-CFB1-4F37-A520-4DA119FA25B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Benötigte Zeit:</t>
   </si>
   <si>
-    <t>Wärmetauscher</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>GJ</t>
+  </si>
+  <si>
+    <t>Wärmepumpe</t>
   </si>
 </sst>
 </file>
@@ -236,20 +236,20 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1793,41 +1793,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="B3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -1835,7 +1835,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="19"/>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1853,17 +1853,17 @@
         <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1874,7 +1874,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1884,25 +1884,25 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="B11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="H11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
@@ -1911,11 +1911,11 @@
         <f>E15*E7/3600*E5</f>
         <v>3530.2499999999991</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="21">
         <f>IF(COUNT(E16,E15,E14,E13)=4,ROUND(E16*E15*(E14-E13),0),"")</f>
         <v>4066848000</v>
       </c>
-      <c r="J12" s="18"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="17">
         <f>IF(COUNT(I12,H12)=2,ROUNDDOWN((I12/H12)/86400,0),"")</f>
         <v>13</v>
@@ -1948,15 +1948,15 @@
         <v>13</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="3">
         <v>30</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>8.0000000000000639</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O14" s="12"/>
     </row>
@@ -1994,7 +1994,7 @@
         <v>4.0668480000000002</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -2024,7 +2024,7 @@
         <v>3.5302499999999992</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -2038,12 +2038,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B15:D15"/>
@@ -2058,6 +2052,12 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated README and LICENSE. Removed hidden data from the Excel spreadsheet. Added the original .svg graphics.
</commit_message>
<xml_diff>
--- a/doc/appendix/Abschaetzung.xlsx
+++ b/doc/appendix/Abschaetzung.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\SwimmingPoolSimulation\doc\appendix\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2EDA93-CFB1-4F37-A520-4DA119FA25B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77201F30-8DF2-443A-833C-28EED2960830}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,20 +231,20 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1793,37 +1788,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
       <c r="L1" s="16"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
@@ -1888,21 +1883,21 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
@@ -1911,11 +1906,11 @@
         <f>E15*E7/3600*E5</f>
         <v>3530.2499999999991</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="18">
         <f>IF(COUNT(E16,E15,E14,E13)=4,ROUND(E16*E15*(E14-E13),0),"")</f>
         <v>4066848000</v>
       </c>
-      <c r="J12" s="21"/>
+      <c r="J12" s="18"/>
       <c r="K12" s="17">
         <f>IF(COUNT(I12,H12)=2,ROUNDDOWN((I12/H12)/86400,0),"")</f>
         <v>13</v>
@@ -1952,11 +1947,11 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="3">
         <v>30</v>
       </c>
@@ -2038,6 +2033,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B15:D15"/>
@@ -2052,12 +2053,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>